<commit_message>
atualização dos artefatos 16 e 17
</commit_message>
<xml_diff>
--- a/17. Análise dos Eventos Para Cada Cenário.xlsx
+++ b/17. Análise dos Eventos Para Cada Cenário.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FreireBreck\Documents\projeto-suellen\Japones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FreireBreck\Documents\projeto-suellen\engenharia-de-requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B9AD9D-E553-421A-9C76-952F6A878FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C368D8-0503-4F13-8CAB-616245E65BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <r>
       <t>Externo</t>
@@ -182,64 +182,16 @@
     <t>x(3)</t>
   </si>
   <si>
-    <t>x(7)</t>
-  </si>
-  <si>
-    <t>Gerar Orçamento</t>
-  </si>
-  <si>
-    <t>Fornecer Produto</t>
-  </si>
-  <si>
-    <t>Logística Reversa</t>
-  </si>
-  <si>
     <t>Cliente solicita o orçamento do produto</t>
   </si>
   <si>
-    <t>Suellen orça o produto solicitado</t>
-  </si>
-  <si>
-    <t>Suellen envia o orçamento para o cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cliente registra o pagamento </t>
-  </si>
-  <si>
-    <t>Suellen valida se a fatura foi paga</t>
-  </si>
-  <si>
-    <t>Suellen envia o produto ao cliente</t>
-  </si>
-  <si>
-    <t>x(4)</t>
-  </si>
-  <si>
-    <t>Cliente solicita o reparo do aparelho</t>
-  </si>
-  <si>
-    <t>Suellen envia orçamento de reparo para cliente fora da garantia</t>
-  </si>
-  <si>
-    <t>Cliente sem garantia autoriza o pagamento da manutenção</t>
-  </si>
-  <si>
     <t>x(9)</t>
   </si>
   <si>
-    <t>x(10)</t>
-  </si>
-  <si>
     <t>FB</t>
   </si>
   <si>
     <t>FA</t>
-  </si>
-  <si>
-    <t>Suellen envia outro produto para o cliente dentro da garantia</t>
-  </si>
-  <si>
-    <t>Suellen envia o produto concertado para cliente sem garantia</t>
   </si>
   <si>
     <r>
@@ -255,6 +207,78 @@
       </rPr>
       <t>*</t>
     </r>
+  </si>
+  <si>
+    <t>Fornecer Orçamento</t>
+  </si>
+  <si>
+    <t>Tratar Venda do Produto</t>
+  </si>
+  <si>
+    <t>Tratar de Configurar Produdo</t>
+  </si>
+  <si>
+    <t>Tratar o Cancelamento do Contrato</t>
+  </si>
+  <si>
+    <t>Tratar a Manutenção do Produto</t>
+  </si>
+  <si>
+    <t>Vendas orça o produto e retorna para o cliente</t>
+  </si>
+  <si>
+    <t>Vendas fecha o contrato e envia para o cliente</t>
+  </si>
+  <si>
+    <t>Fábrica inicia a produção do produto</t>
+  </si>
+  <si>
+    <t>Assistência envia o produto configurado para o cliente</t>
+  </si>
+  <si>
+    <t>Cliente solicita o cancelamento do contrato</t>
+  </si>
+  <si>
+    <t>Assistência inicia o processo de cancelamento</t>
+  </si>
+  <si>
+    <t>Cliente envia um feedback sobre o produto</t>
+  </si>
+  <si>
+    <t>Cliente solicita a manutenção do produto</t>
+  </si>
+  <si>
+    <t>Assistência gera o orçamento da manutenção</t>
+  </si>
+  <si>
+    <t>Assistência valida a garantia do produto</t>
+  </si>
+  <si>
+    <t>Assistência realiza o concerto do produto</t>
+  </si>
+  <si>
+    <t>Cliente recebe produto em perfeito estado</t>
+  </si>
+  <si>
+    <t>Cliente envia solicitação de compra</t>
+  </si>
+  <si>
+    <t>Fábrica envia o produto com configurações base</t>
+  </si>
+  <si>
+    <t>Banco envia extrato de pagamento da fatura</t>
+  </si>
+  <si>
+    <t>x(5)</t>
+  </si>
+  <si>
+    <t>x(6)</t>
+  </si>
+  <si>
+    <t>x(12)</t>
+  </si>
+  <si>
+    <t>x(13)</t>
   </si>
 </sst>
 </file>
@@ -290,7 +314,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +357,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -389,15 +425,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -513,17 +540,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -556,11 +572,22 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,7 +599,7 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -582,18 +609,7 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -606,19 +622,21 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -638,80 +656,95 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1052,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,26 +1102,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="19" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="19" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="9"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1096,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
@@ -1110,22 +1143,22 @@
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>29</v>
+      <c r="A3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
@@ -1134,16 +1167,16 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="11"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1152,192 +1185,298 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="7">
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="6">
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="11"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="3">
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="3">
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="6">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>29</v>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="3">
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="6">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="29" t="s">
-        <v>30</v>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="C11" s="3">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="11"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="3">
+      <c r="A12" s="29"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="6">
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="31"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="C13" s="3">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="F13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="11"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="3">
+        <v>13</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="3">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="B18" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A6:A8"/>
+  <mergeCells count="15">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A9:A13"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A3:A4"/>
     <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
alteração 16, 20 e 21
</commit_message>
<xml_diff>
--- a/17. Análise dos Eventos Para Cada Cenário.xlsx
+++ b/17. Análise dos Eventos Para Cada Cenário.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FreireBreck\Documents\projeto-suellen\engenharia-de-requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C368D8-0503-4F13-8CAB-616245E65BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFCB712-DDFA-43CA-8599-E8102308F09C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -671,6 +671,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -680,12 +728,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -703,48 +745,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,25 +1103,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="18"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1148,10 +1148,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="6">
@@ -1170,8 +1170,8 @@
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -1188,7 +1188,7 @@
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -1210,7 +1210,7 @@
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="26"/>
       <c r="C6" s="6">
         <v>4</v>
@@ -1228,7 +1228,7 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="26"/>
       <c r="C7" s="3">
         <v>5</v>
@@ -1246,7 +1246,7 @@
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="27"/>
       <c r="C8" s="6">
         <v>6</v>
@@ -1264,7 +1264,7 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -1286,7 +1286,7 @@
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="27"/>
       <c r="C10" s="6">
         <v>8</v>
@@ -1304,7 +1304,7 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -1326,7 +1326,7 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="27"/>
       <c r="C12" s="6">
         <v>10</v>
@@ -1344,7 +1344,7 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="11" t="s">
         <v>16</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -1386,7 +1386,7 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="27"/>
       <c r="C15" s="3">
         <v>13</v>
@@ -1404,7 +1404,7 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="25" t="s">
         <v>16</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="27"/>
       <c r="C17" s="3">
         <v>15</v>
@@ -1442,8 +1442,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="37" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="6">
@@ -1463,6 +1463,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A4"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="A5:A8"/>
@@ -1472,11 +1477,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A4"/>
     <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>